<commit_message>
Ajustes para gerar dados para o artigo extendido
</commit_message>
<xml_diff>
--- a/data/Datas Versoes.xlsx
+++ b/data/Datas Versoes.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$D$25</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>apache-ant-1.5.2-bin.zip</t>
   </si>
@@ -218,6 +219,18 @@
   </si>
   <si>
     <t>apache-ant-1.3.0</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>MQ</t>
+  </si>
+  <si>
+    <t>EVM</t>
   </si>
 </sst>
 </file>
@@ -267,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -277,6 +290,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,7 +594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -611,7 +627,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="1">
-        <v>37845</v>
+        <v>36726</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>27</v>
@@ -625,7 +641,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="1">
-        <v>37845</v>
+        <v>36823</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -639,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1">
-        <v>37845</v>
+        <v>36953</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>31</v>
@@ -653,7 +669,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="1">
-        <v>37845</v>
+        <v>37137</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
@@ -667,7 +683,7 @@
         <v>34</v>
       </c>
       <c r="C6" s="1">
-        <v>37845</v>
+        <v>37175</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>33</v>
@@ -681,7 +697,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="1">
-        <v>37845</v>
+        <v>37447</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
@@ -695,7 +711,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="1">
-        <v>37845</v>
+        <v>37532</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>38</v>
@@ -709,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>37845</v>
+        <v>37683</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>1</v>
@@ -723,7 +739,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>37727</v>
+        <v>37720</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
@@ -948,4 +964,515 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1">
+        <v>36726</v>
+      </c>
+      <c r="C2">
+        <v>102</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5">
+        <v>17912</v>
+      </c>
+      <c r="F2">
+        <v>-1867</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1">
+        <v>36823</v>
+      </c>
+      <c r="C3">
+        <v>173</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5">
+        <v>41135</v>
+      </c>
+      <c r="F3">
+        <v>-4011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="1">
+        <v>36953</v>
+      </c>
+      <c r="C4">
+        <v>187</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>40193</v>
+      </c>
+      <c r="F4">
+        <v>-4843</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <v>37137</v>
+      </c>
+      <c r="C5">
+        <v>265</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5">
+        <v>58274</v>
+      </c>
+      <c r="F5">
+        <v>-8443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="1">
+        <v>37175</v>
+      </c>
+      <c r="C6">
+        <v>265</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5">
+        <v>58512</v>
+      </c>
+      <c r="F6">
+        <v>-8441</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1">
+        <v>37447</v>
+      </c>
+      <c r="C7">
+        <v>401</v>
+      </c>
+      <c r="D7">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5">
+        <v>98538</v>
+      </c>
+      <c r="F7">
+        <v>-13471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1">
+        <v>37532</v>
+      </c>
+      <c r="C8">
+        <v>401</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5">
+        <v>98518</v>
+      </c>
+      <c r="F8">
+        <v>-13471</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1">
+        <v>37683</v>
+      </c>
+      <c r="C9">
+        <v>406</v>
+      </c>
+      <c r="D9">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5">
+        <v>98362</v>
+      </c>
+      <c r="F9">
+        <v>-13855</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1">
+        <v>37720</v>
+      </c>
+      <c r="C10">
+        <v>407</v>
+      </c>
+      <c r="D10">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5">
+        <v>98359</v>
+      </c>
+      <c r="F10">
+        <v>-14008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="1">
+        <v>37845</v>
+      </c>
+      <c r="C11">
+        <v>407</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+      <c r="E11" s="5">
+        <v>98359</v>
+      </c>
+      <c r="F11">
+        <v>-14008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1">
+        <v>37973</v>
+      </c>
+      <c r="C12">
+        <v>523</v>
+      </c>
+      <c r="D12">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5">
+        <v>109383</v>
+      </c>
+      <c r="F12">
+        <v>-21519</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1">
+        <v>38029</v>
+      </c>
+      <c r="C13">
+        <v>524</v>
+      </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+      <c r="E13" s="5">
+        <v>109411</v>
+      </c>
+      <c r="F13">
+        <v>-21664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1">
+        <v>38184</v>
+      </c>
+      <c r="C14">
+        <v>553</v>
+      </c>
+      <c r="D14">
+        <v>24</v>
+      </c>
+      <c r="E14" s="5">
+        <v>113280</v>
+      </c>
+      <c r="F14">
+        <v>-24526</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1">
+        <v>38470</v>
+      </c>
+      <c r="C15">
+        <v>576</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15" s="5">
+        <v>112216</v>
+      </c>
+      <c r="F15">
+        <v>-27430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1">
+        <v>38491</v>
+      </c>
+      <c r="C16">
+        <v>576</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16" s="5">
+        <v>112216</v>
+      </c>
+      <c r="F16">
+        <v>-27430</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1">
+        <v>38505</v>
+      </c>
+      <c r="C17">
+        <v>576</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17" s="5">
+        <v>112202</v>
+      </c>
+      <c r="F17">
+        <v>-27430</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1">
+        <v>39064</v>
+      </c>
+      <c r="C18">
+        <v>752</v>
+      </c>
+      <c r="D18">
+        <v>29</v>
+      </c>
+      <c r="E18" s="5">
+        <v>117711</v>
+      </c>
+      <c r="F18">
+        <v>-39057</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="1">
+        <v>39638</v>
+      </c>
+      <c r="C19">
+        <v>769</v>
+      </c>
+      <c r="D19">
+        <v>29</v>
+      </c>
+      <c r="E19" s="5">
+        <v>121425</v>
+      </c>
+      <c r="F19">
+        <v>-40263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="1">
+        <v>40211</v>
+      </c>
+      <c r="C20">
+        <v>870</v>
+      </c>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20" s="5">
+        <v>125600</v>
+      </c>
+      <c r="F20">
+        <v>-49381</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="1">
+        <v>40298</v>
+      </c>
+      <c r="C21">
+        <v>873</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
+      <c r="E21" s="5">
+        <v>126022</v>
+      </c>
+      <c r="F21">
+        <v>-49629</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1">
+        <v>40532</v>
+      </c>
+      <c r="C22">
+        <v>1090</v>
+      </c>
+      <c r="D22">
+        <v>59</v>
+      </c>
+      <c r="E22" s="5">
+        <v>213681</v>
+      </c>
+      <c r="F22">
+        <v>-51615</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="1">
+        <v>40981</v>
+      </c>
+      <c r="C23">
+        <v>1093</v>
+      </c>
+      <c r="D23">
+        <v>59</v>
+      </c>
+      <c r="E23" s="5">
+        <v>213193</v>
+      </c>
+      <c r="F23">
+        <v>-51828</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41052</v>
+      </c>
+      <c r="C24">
+        <v>1094</v>
+      </c>
+      <c r="D24">
+        <v>59</v>
+      </c>
+      <c r="E24" s="5">
+        <v>213777</v>
+      </c>
+      <c r="F24">
+        <v>-51830</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41343</v>
+      </c>
+      <c r="C25">
+        <v>1116</v>
+      </c>
+      <c r="D25">
+        <v>60</v>
+      </c>
+      <c r="E25" s="5">
+        <v>220524</v>
+      </c>
+      <c r="F25">
+        <v>-49639</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>